<commit_message>
update functional with excel
</commit_message>
<xml_diff>
--- a/model/data/table1.xlsx
+++ b/model/data/table1.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H3"/>
+  <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,172 @@
       <c r="G3" s="2" t="n"/>
       <c r="H3" s="2" t="n"/>
     </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>13-Oct</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>АОР</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Посев</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Ячмень яровой</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>420</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>14-Oct</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Центральное</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Уборка</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Кукуруза</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>3150</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>18700</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>12-Oct</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>АОР</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Внесение минеральных удобрений</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Пшеница озимая</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>149</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>7264</v>
+      </c>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>13-Oct</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>АОР</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Посев</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Ячмень яровой</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>420</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>14-Oct</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Центральное</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Уборка</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Кукуруза</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>3150</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>18700</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>